<commit_message>
Update headlines to top 150
</commit_message>
<xml_diff>
--- a/datastore/headline.xlsx
+++ b/datastore/headline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>headline</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -199,6 +199,635 @@
   </si>
   <si>
     <t>경향</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플라자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책의 향기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유레카</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간추린 뉴스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세상 읽기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Health&amp;Beauty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>글로벌 콕콕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Money&amp;Life</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데스크에서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>땅, 땅… 오늘의 판결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배달의 한겨레</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LG배 조선일보 기왕전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동서남북</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>독자 마당</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통일나눔펀드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기업&amp;CEO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인물동정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여행, 나를 찾아서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골든걸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>윤희영의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> News English</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뉴스파일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한겨레 프리즘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로컬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴스</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태평로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기자의 시각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조선일보를 읽고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아침 햇발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>편집국에서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책속의 이 한줄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한겨레 사설</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>렌즈세상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문화 소식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEWS&amp;VIEW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헬스&amp;뷰티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뉴스 TALK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Love&amp;Gift</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q매거진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전문기자 칼럼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>권혁웅의 오목렌즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가슴으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>읽는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>동시</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESSAY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특파원 칼럼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경제포커스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월드 톡톡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김대식의 브레인 스토리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가슴으로 읽는 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가슴으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>읽는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시조</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가슴으로 읽는 한시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최재천의 자연과 문화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>편집자 레터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삶의 창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사설 속으로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세계의 창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>함께</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>읽는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>동아일보</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특파원 리포트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기자수첩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트렌드 돋보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신의 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정훈이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>만화</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>최보식이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>만난</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사람</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미래로 뛰는 한국기업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포토에세이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2030 잠금해제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신문은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선생님</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R&amp;D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>희망이다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금주의 공연, 이유 있는 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠깐만요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바로잡습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타인의 시선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와!글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미디어 전망대</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -206,7 +835,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +850,19 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -584,13 +1226,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -813,8 +1455,399 @@
         <v>43</v>
       </c>
     </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update clustering final script
</commit_message>
<xml_diff>
--- a/datastore/headline.xlsx
+++ b/datastore/headline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>headline</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -290,28 +290,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>윤희영의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> News English</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>뉴스파일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -320,38 +298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>로컬</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>뉴스</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>태평로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -428,57 +374,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>가슴으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>읽는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>동시</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ESSAY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -503,57 +398,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>가슴으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>읽는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>시조</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>가슴으로 읽는 한시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -578,57 +422,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>함께</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>읽는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>동아일보</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>특파원 리포트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -645,89 +438,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>정훈이</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>만화</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>최보식이</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>만난</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사람</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>미래로 뛰는 한국기업</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -740,73 +450,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>신문은</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>선생님</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>R&amp;D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>가</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>희망이다</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>금주의 공연, 이유 있는 선택</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -828,6 +471,46 @@
   </si>
   <si>
     <t>미디어 전망대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 역사다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>함께 읽는 동아일보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신문은 선생님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R&amp;D가 희망이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가슴으로 읽는 시조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정훈이 만화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최보식이 만난 사람</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가슴으로 읽는 동시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로컬 뉴스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤희영의 News English</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -835,7 +518,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,19 +533,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1226,7 +896,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A122"/>
+  <dimension ref="A1:A123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1572,277 +1242,282 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>